<commit_message>
Realizacion del documento de levantamineto de la informacion
</commit_message>
<xml_diff>
--- a/App/app_documentacion/1er_trimestre/3_recoleccion/1_3_1_recoleccion_informacion (2).xlsx
+++ b/App/app_documentacion/1er_trimestre/3_recoleccion/1_3_1_recoleccion_informacion (2).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEACA6F0-3266-4953-82B9-3F16ADECCC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91894456-6B3D-4273-98B3-4F6FF215BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
   <si>
     <t>HOJA DE CONTROL</t>
   </si>
@@ -386,6 +386,33 @@
   </si>
   <si>
     <t>Aaron Sierra (Colaborador 2)</t>
+  </si>
+  <si>
+    <t>Diagrama de Procesos</t>
+  </si>
+  <si>
+    <t>&lt;Aaron Sierra&gt;</t>
+  </si>
+  <si>
+    <t>14/11/2021</t>
+  </si>
+  <si>
+    <t>Documento formulacion de proyecto</t>
+  </si>
+  <si>
+    <t>&lt;Brayan Rosas&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentación del proyecto </t>
+  </si>
+  <si>
+    <t>Levantamiento de la información</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>&lt;Katerine Morcillo&gt; &lt;Brayan Rosas&gt;</t>
   </si>
 </sst>
 </file>
@@ -781,36 +808,6 @@
         <color rgb="FF999999"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF999999"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF999999"/>
       </bottom>
       <diagonal/>
@@ -1096,13 +1093,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1165,12 +1188,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1178,9 +1195,9 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1191,57 +1208,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1252,13 +1269,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1268,71 +1285,78 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2385,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:IV89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B46" sqref="B7:F46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2411,44 +2435,44 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="2:8" ht="30">
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="80"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="71"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="30">
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="12" spans="2:8">
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="30">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1">
       <c r="B17" s="2"/>
@@ -2459,54 +2483,54 @@
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
     </row>
     <row r="19" spans="2:16" ht="18">
       <c r="B19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
     </row>
     <row r="20" spans="2:16" ht="18">
       <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="83" t="s">
+      <c r="C20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
     </row>
     <row r="21" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="85"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="8" t="s">
         <v>7</v>
       </c>
@@ -2518,10 +2542,10 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="70"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="10" t="s">
         <v>9</v>
       </c>
@@ -2529,8 +2553,8 @@
     </row>
     <row r="24" spans="2:16" ht="36.75" thickBot="1">
       <c r="B24" s="11"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="12" t="s">
         <v>10</v>
       </c>
@@ -2558,10 +2582,10 @@
       <c r="C28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="73" t="s">
+      <c r="D28" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="73"/>
+      <c r="E28" s="79"/>
       <c r="F28" s="18" t="s">
         <v>16</v>
       </c>
@@ -2573,448 +2597,502 @@
       <c r="C29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="74" t="s">
+      <c r="D29" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="74"/>
+      <c r="E29" s="80"/>
       <c r="F29" s="21" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="9"/>
+      <c r="B30" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="91"/>
+      <c r="F30" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="39" customHeight="1">
+      <c r="B31" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="91" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="91"/>
+      <c r="F31" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="32" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="13"/>
-    </row>
-    <row r="38" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="B32" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="93"/>
+      <c r="F32" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:256" ht="40.5" customHeight="1">
+      <c r="B33" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="93"/>
+      <c r="F33" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:256" ht="25.5" customHeight="1">
+      <c r="B34" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="93"/>
+      <c r="F34" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:256" ht="25.5" customHeight="1">
+      <c r="IR35" s="2"/>
+      <c r="IS35" s="2"/>
+      <c r="IT35" s="2"/>
+      <c r="IU35" s="2"/>
+      <c r="IV35" s="2"/>
+    </row>
+    <row r="36" spans="1:256" ht="25.5" customHeight="1">
+      <c r="IR36" s="2"/>
+      <c r="IS36" s="2"/>
+      <c r="IT36" s="2"/>
+      <c r="IU36" s="2"/>
+      <c r="IV36" s="2"/>
+    </row>
+    <row r="37" spans="1:256" ht="25.5" customHeight="1">
+      <c r="IR37" s="2"/>
+      <c r="IS37" s="2"/>
+      <c r="IT37" s="2"/>
+      <c r="IU37" s="2"/>
+      <c r="IV37" s="2"/>
+    </row>
+    <row r="38" spans="1:256" ht="19.899999999999999" customHeight="1">
       <c r="A38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="19.899999999999999" customHeight="1">
+    <row r="39" spans="1:256" ht="19.899999999999999" customHeight="1">
       <c r="B39" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="30" customHeight="1" thickBot="1"/>
-    <row r="41" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B41" s="72" t="s">
+    <row r="40" spans="1:256" ht="30" customHeight="1" thickBot="1"/>
+    <row r="41" spans="1:256" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B41" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-    </row>
-    <row r="42" spans="1:10" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B42" s="69" t="s">
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+    </row>
+    <row r="42" spans="1:256" ht="25.5" customHeight="1" thickTop="1">
+      <c r="B42" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-    </row>
-    <row r="43" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B43" s="70" t="s">
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="81"/>
+    </row>
+    <row r="43" spans="1:256" ht="25.5" customHeight="1">
+      <c r="B43" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
       <c r="J43" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B44" s="70" t="s">
+    <row r="44" spans="1:256" ht="25.5" customHeight="1">
+      <c r="B44" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-    </row>
-    <row r="45" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B45" s="70"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="26"/>
-    </row>
-    <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B46" s="71"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="71"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="71"/>
-    </row>
-    <row r="47" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="26"/>
-    </row>
-    <row r="48" spans="1:10" ht="19.899999999999999" customHeight="1">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+    </row>
+    <row r="45" spans="1:256" ht="25.5" customHeight="1">
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:256" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B46" s="78"/>
+      <c r="C46" s="78"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+    </row>
+    <row r="47" spans="1:256" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="24"/>
+    </row>
+    <row r="48" spans="1:256" ht="19.899999999999999" customHeight="1">
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" spans="1:13" ht="19.899999999999999" customHeight="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="27"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="26"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="26"/>
+      <c r="F49" s="24"/>
       <c r="G49" s="2"/>
-      <c r="I49" s="29"/>
+      <c r="I49" s="27"/>
     </row>
     <row r="50" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
     </row>
     <row r="51" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A51" s="27"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
     </row>
     <row r="52" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
       <c r="G52" s="2"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
     </row>
     <row r="53" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="30"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="28"/>
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
     </row>
     <row r="54" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="26"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="24"/>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
     </row>
     <row r="55" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A55" s="31"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
     </row>
     <row r="56" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
     </row>
     <row r="57" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A57" s="31"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
       <c r="K57" s="15"/>
       <c r="L57" s="15"/>
     </row>
     <row r="58" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="F58" s="34"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="F58" s="32"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
     </row>
     <row r="59" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="G59" s="26"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="G59" s="24"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
     </row>
     <row r="60" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="F60" s="28"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="F60" s="26"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
     </row>
     <row r="61" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="28"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="26"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
     </row>
     <row r="62" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="28"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="26"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
     </row>
     <row r="63" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="26"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="24"/>
       <c r="K63" s="15"/>
       <c r="L63" s="15"/>
     </row>
     <row r="64" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="26"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="24"/>
       <c r="K64" s="15"/>
       <c r="L64" s="15"/>
     </row>
     <row r="65" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A65" s="31"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="G65" s="26"/>
+      <c r="A65" s="29"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="G65" s="24"/>
       <c r="K65" s="15"/>
       <c r="L65" s="15"/>
     </row>
     <row r="66" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A66" s="31"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
+      <c r="A66" s="29"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
     </row>
     <row r="67" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
+      <c r="A67" s="29"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
     </row>
     <row r="68" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A68" s="31"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
+      <c r="A68" s="29"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A69" s="31"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
     </row>
     <row r="70" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A70" s="31"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="26"/>
+      <c r="A70" s="29"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
     </row>
     <row r="71" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
+      <c r="A71" s="29"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
     </row>
     <row r="72" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
+      <c r="A72" s="29"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
     </row>
     <row r="73" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
+      <c r="A73" s="29"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
     </row>
     <row r="74" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
     </row>
     <row r="75" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
+      <c r="A75" s="29"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
     </row>
     <row r="76" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
     </row>
     <row r="77" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="B77" s="35"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
     </row>
     <row r="78" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
     </row>
     <row r="79" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="B79" s="35"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
     </row>
     <row r="80" spans="1:12" ht="19.899999999999999" customHeight="1">
-      <c r="B80" s="26"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-      <c r="J80" s="36"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="J80" s="34"/>
     </row>
     <row r="81" spans="2:10">
-      <c r="B81" s="35"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="J81" s="36"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="J81" s="34"/>
     </row>
     <row r="82" spans="2:10">
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
     </row>
     <row r="83" spans="2:10">
-      <c r="B83" s="35"/>
-      <c r="C83" s="26"/>
-      <c r="D83" s="26"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
     </row>
     <row r="84" spans="2:10">
-      <c r="B84" s="26"/>
-      <c r="C84" s="26"/>
-      <c r="D84" s="26"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
     </row>
     <row r="85" spans="2:10">
-      <c r="B85" s="35"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
     </row>
     <row r="86" spans="2:10">
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
     </row>
     <row r="87" spans="2:10">
-      <c r="B87" s="35"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
+      <c r="B87" s="33"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
     </row>
     <row r="88" spans="2:10">
-      <c r="B88" s="28"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
     </row>
     <row r="89" spans="2:10">
-      <c r="C89" s="28"/>
-      <c r="D89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="26">
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
@@ -3027,23 +3105,6 @@
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.9763779527559107E-2" bottom="3.9763779527559107E-2" header="0" footer="0"/>
@@ -3079,382 +3140,382 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:9">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="2:9" ht="30">
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="80"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
     </row>
     <row r="8" spans="2:9" ht="30">
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="80"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-    </row>
-    <row r="11" spans="2:9" s="37" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="B11" s="47" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="2:9" s="35" customFormat="1" ht="24" customHeight="1" thickBot="1">
+      <c r="B11" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="49" t="s">
+      <c r="I11" s="47" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="40" customFormat="1" ht="37.5" customHeight="1">
-      <c r="B12" s="88" t="s">
+    <row r="12" spans="2:9" s="38" customFormat="1" ht="37.5" customHeight="1">
+      <c r="B12" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="52">
         <v>44536</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="57" t="s">
+      <c r="I12" s="55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:9" s="40" customFormat="1" ht="42" customHeight="1">
-      <c r="B13" s="89"/>
-      <c r="C13" s="38" t="s">
+    <row r="13" spans="2:9" s="38" customFormat="1" ht="42" customHeight="1">
+      <c r="B13" s="85"/>
+      <c r="C13" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="53">
         <v>44536</v>
       </c>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="56" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="2:9" customFormat="1" ht="45">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="52">
         <v>44536</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="39"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="2:9" customFormat="1" ht="51.75" customHeight="1">
-      <c r="B15" s="89"/>
-      <c r="C15" s="38" t="s">
+      <c r="B15" s="85"/>
+      <c r="C15" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="52">
         <v>44536</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="39"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="16" spans="2:9" customFormat="1" ht="43.5" customHeight="1">
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="53">
         <v>44536</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:256" customFormat="1" ht="27" customHeight="1">
-      <c r="B17" s="87"/>
-      <c r="C17" s="38" t="s">
+      <c r="B17" s="83"/>
+      <c r="C17" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="52">
         <v>44536</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="41"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:256" customFormat="1" ht="15">
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="1:256" customFormat="1" ht="15">
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="1:256" customFormat="1" ht="15">
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
       <c r="IV21" s="2"/>
     </row>
     <row r="22" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="IV22" s="2"/>
     </row>
     <row r="23" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="IV23" s="2"/>
     </row>
     <row r="24" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="IV24" s="2"/>
     </row>
     <row r="25" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="IV25" s="2"/>
     </row>
     <row r="26" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="IV26" s="2"/>
     </row>
     <row r="27" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="IV27" s="2"/>
     </row>
     <row r="28" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="IV28" s="2"/>
     </row>
     <row r="29" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IV29" s="2"/>
     </row>
     <row r="30" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IV30" s="2"/>
     </row>
     <row r="31" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IV31" s="2"/>
     </row>
     <row r="32" spans="1:256" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="I32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="I32" s="34"/>
       <c r="IV32" s="2"/>
     </row>
     <row r="33" spans="2:256" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="I33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="I33" s="34"/>
       <c r="IV33" s="2"/>
     </row>
     <row r="34" spans="2:256" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IV34" s="2"/>
     </row>
     <row r="35" spans="2:256" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IV35" s="2"/>
     </row>
     <row r="36" spans="2:256" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IV36" s="2"/>
     </row>
     <row r="37" spans="2:256" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IV37" s="2"/>
     </row>
     <row r="38" spans="2:256" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IV38" s="2"/>
     </row>
     <row r="39" spans="2:256" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IV39" s="2"/>
     </row>
     <row r="40" spans="2:256" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IV40" s="2"/>
     </row>
     <row r="41" spans="2:256" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IV41" s="2"/>
     </row>
   </sheetData>
@@ -3505,236 +3566,236 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:257" ht="30">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="48"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
       <c r="F7" s="3"/>
     </row>
     <row r="9" spans="1:257" ht="114">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="66" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:257" ht="71.25">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="66" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:257">
-      <c r="B11" s="68"/>
+      <c r="B11" s="66"/>
     </row>
     <row r="12" spans="1:257">
-      <c r="B12" s="68"/>
+      <c r="B12" s="66"/>
       <c r="F12" s="4"/>
     </row>
     <row r="14" spans="1:257" ht="9.75" customHeight="1"/>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="IW15" s="2"/>
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="IW17" s="2"/>
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="IW18" s="2"/>
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="IW22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="IW24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" spans="2:257" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" spans="2:257" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" spans="2:257" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" spans="2:257" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" spans="2:257" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" spans="2:257" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IW41" s="2"/>
     </row>
   </sheetData>
@@ -3781,340 +3842,340 @@
       <c r="F2" s="2"/>
     </row>
     <row r="4" spans="1:257" ht="30">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="80"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:257" ht="30.75" customHeight="1">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="33.75" customHeight="1">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:257" ht="409.5">
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="64" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:257" ht="15">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:257" ht="15.75" thickBot="1">
-      <c r="B12" s="61"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:257" ht="15" thickBot="1">
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="63" t="s">
+      <c r="D13" s="90"/>
+      <c r="E13" s="61" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:257" ht="15" thickBot="1">
-      <c r="B14" s="92"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="64"/>
+      <c r="E14" s="62"/>
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="99.75" customHeight="1" thickBot="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="65" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64" t="s">
+      <c r="D15" s="62"/>
+      <c r="E15" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="IW15" s="2"/>
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="65" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64" t="s">
+      <c r="D16" s="62"/>
+      <c r="E16" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="65" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="G17" s="26"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="G17" s="24"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="IW17" s="2"/>
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="65" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64" t="s">
+      <c r="C18" s="62"/>
+      <c r="D18" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="64"/>
+      <c r="E18" s="62"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="IW18" s="2"/>
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="65" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="64" t="s">
+      <c r="E20" s="62" t="s">
         <v>72</v>
       </c>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="65" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64" t="s">
+      <c r="C21" s="62"/>
+      <c r="D21" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="64" t="s">
+      <c r="E21" s="62" t="s">
         <v>74</v>
       </c>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="65" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
       <c r="IW22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="65" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="64"/>
+      <c r="E23" s="62"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="65" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64" t="s">
+      <c r="C24" s="62"/>
+      <c r="D24" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="64"/>
+      <c r="E24" s="62"/>
       <c r="IW24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="65" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64" t="s">
+      <c r="D25" s="62"/>
+      <c r="E25" s="62" t="s">
         <v>79</v>
       </c>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="65" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64" t="s">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="64"/>
+      <c r="E26" s="62"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="65" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" spans="2:257" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" spans="2:257" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" spans="2:257" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" spans="2:257" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" spans="2:257" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" spans="2:257" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IW41" s="2"/>
     </row>
   </sheetData>
@@ -4164,36 +4225,36 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71"/>
     </row>
     <row r="9" spans="1:257" ht="24.75" customHeight="1"/>
     <row r="10" spans="1:257" ht="409.5">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="57" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4201,194 +4262,194 @@
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="IW15" s="2"/>
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="IW17" s="2"/>
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="IW18" s="2"/>
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="IW22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="IW24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" spans="2:257" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" spans="2:257" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" spans="2:257" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" spans="2:257" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" spans="2:257" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" spans="2:257" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IW41" s="2"/>
     </row>
   </sheetData>
@@ -4435,225 +4496,225 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="80"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="71"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="IW15" s="2"/>
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="IW17" s="2"/>
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="IW18" s="2"/>
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="IW22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="IW24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" spans="2:257" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" spans="2:257" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" spans="2:257" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" spans="2:257" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" spans="2:257" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" spans="2:257" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IW41" s="2"/>
     </row>
   </sheetData>
@@ -4701,27 +4762,27 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:257" ht="30">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="71"/>
     </row>
     <row r="5" spans="1:257" ht="30">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:257" ht="30">
       <c r="F7" s="3"/>
@@ -4730,194 +4791,194 @@
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="IW15" s="2"/>
     </row>
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="IW16" s="2"/>
     </row>
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="IW17" s="2"/>
     </row>
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="IW18" s="2"/>
     </row>
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="IW19" s="2"/>
     </row>
     <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="IW22" s="2"/>
     </row>
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="IW24" s="2"/>
     </row>
     <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
       <c r="IW31" s="2"/>
     </row>
     <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="J32" s="34"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" spans="2:257" s="1" customFormat="1">
-      <c r="B33" s="35"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="J33" s="34"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" spans="2:257" s="1" customFormat="1">
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" spans="2:257" s="1" customFormat="1">
-      <c r="B35" s="35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" spans="2:257" s="1" customFormat="1">
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" spans="2:257" s="1" customFormat="1">
-      <c r="B37" s="35"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" spans="2:257" s="1" customFormat="1">
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" spans="2:257" s="1" customFormat="1">
-      <c r="B39" s="35"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" spans="2:257" s="1" customFormat="1">
-      <c r="B40" s="28"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" spans="2:257" s="1" customFormat="1">
-      <c r="C41" s="28"/>
-      <c r="D41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="24"/>
       <c r="IW41" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego actividades de 2do trimestre
</commit_message>
<xml_diff>
--- a/App/app_documentacion/1er_trimestre/3_recoleccion/1_3_1_recoleccion_informacion (2).xlsx
+++ b/App/app_documentacion/1er_trimestre/3_recoleccion/1_3_1_recoleccion_informacion (2).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91894456-6B3D-4273-98B3-4F6FF215BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA86FEC-E3FA-4B39-B39D-830B27D43081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>Katherine Morcillo</t>
-  </si>
-  <si>
-    <t>Describir como se hace el marketing dentro de la empresa</t>
   </si>
   <si>
     <t xml:space="preserve">Lista de Chequeo </t>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>&lt;Katerine Morcillo&gt; &lt;Brayan Rosas&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conocer cómo se realizan las ventas en la empresa </t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1285,27 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,17 +1331,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1348,15 +1357,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2409,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:IV89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:F44"/>
     </sheetView>
   </sheetViews>
@@ -2435,44 +2435,44 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="2:8" ht="30">
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="71"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="30">
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="71"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="79"/>
     </row>
     <row r="12" spans="2:8">
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="30">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1">
       <c r="B17" s="2"/>
@@ -2483,54 +2483,54 @@
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
     </row>
     <row r="19" spans="2:16" ht="18">
       <c r="B19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
     </row>
     <row r="20" spans="2:16" ht="18">
       <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
     </row>
     <row r="21" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="76"/>
+      <c r="D22" s="84"/>
       <c r="E22" s="8" t="s">
         <v>7</v>
       </c>
@@ -2542,10 +2542,10 @@
       <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="67"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="10" t="s">
         <v>9</v>
       </c>
@@ -2553,8 +2553,8 @@
     </row>
     <row r="24" spans="2:16" ht="36.75" thickBot="1">
       <c r="B24" s="11"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
       <c r="E24" s="12" t="s">
         <v>10</v>
       </c>
@@ -2582,10 +2582,10 @@
       <c r="C28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="79" t="s">
+      <c r="D28" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="79"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="18" t="s">
         <v>16</v>
       </c>
@@ -2595,14 +2595,14 @@
         <v>6</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="72"/>
+      <c r="F29" s="21" t="s">
         <v>87</v>
-      </c>
-      <c r="E29" s="80"/>
-      <c r="F29" s="21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1">
@@ -2610,14 +2610,14 @@
         <v>6</v>
       </c>
       <c r="C30" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="E30" s="73"/>
+      <c r="F30" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="E30" s="91"/>
-      <c r="F30" s="9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="39" customHeight="1">
@@ -2625,14 +2625,14 @@
         <v>6</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="91" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="91"/>
+      <c r="E31" s="73"/>
       <c r="F31" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="25.5" customHeight="1">
@@ -2640,14 +2640,14 @@
         <v>6</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="92" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="93"/>
+        <v>97</v>
+      </c>
+      <c r="D32" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="75"/>
       <c r="F32" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:256" ht="40.5" customHeight="1">
@@ -2655,14 +2655,14 @@
         <v>6</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="92" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="93"/>
+        <v>98</v>
+      </c>
+      <c r="D33" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="75"/>
       <c r="F33" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:256" ht="25.5" customHeight="1">
@@ -2670,14 +2670,14 @@
         <v>6</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="92" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="93"/>
+        <v>99</v>
+      </c>
+      <c r="D34" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="75"/>
       <c r="F34" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:256" ht="25.5" customHeight="1">
@@ -2712,58 +2712,58 @@
     </row>
     <row r="40" spans="1:256" ht="30" customHeight="1" thickBot="1"/>
     <row r="41" spans="1:256" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B41" s="77" t="s">
+      <c r="B41" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
     </row>
     <row r="42" spans="1:256" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B42" s="81" t="s">
+      <c r="B42" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+    </row>
+    <row r="43" spans="1:256" ht="25.5" customHeight="1">
+      <c r="B43" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-    </row>
-    <row r="43" spans="1:256" ht="25.5" customHeight="1">
-      <c r="B43" s="67" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
       <c r="J43" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:256" ht="25.5" customHeight="1">
-      <c r="B44" s="67" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="67"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="67"/>
+      <c r="B44" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
     </row>
     <row r="45" spans="1:256" ht="25.5" customHeight="1">
-      <c r="B45" s="67"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
       <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:256" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B46" s="78"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="78"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
     </row>
     <row r="47" spans="1:256" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A47" s="25"/>
@@ -3079,20 +3079,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
@@ -3105,6 +3091,20 @@
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.9763779527559107E-2" bottom="3.9763779527559107E-2" header="0" footer="0"/>
@@ -3117,8 +3117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:IV41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3140,36 +3140,36 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:9">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="2:9" ht="30">
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
     </row>
     <row r="8" spans="2:9" ht="30">
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="79"/>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1">
       <c r="B10" s="40"/>
@@ -3208,7 +3208,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" s="38" customFormat="1" ht="37.5" customHeight="1">
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="87" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="44" t="s">
@@ -3234,7 +3234,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" s="38" customFormat="1" ht="42" customHeight="1">
-      <c r="B13" s="85"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="36" t="s">
         <v>39</v>
       </c>
@@ -3258,7 +3258,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" customFormat="1" ht="45">
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="89" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -3282,7 +3282,7 @@
       <c r="I14" s="37"/>
     </row>
     <row r="15" spans="2:9" customFormat="1" ht="51.75" customHeight="1">
-      <c r="B15" s="85"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="36" t="s">
         <v>39</v>
       </c>
@@ -3304,8 +3304,8 @@
       <c r="I15" s="37"/>
     </row>
     <row r="16" spans="2:9" customFormat="1" ht="43.5" customHeight="1">
-      <c r="B16" s="82" t="s">
-        <v>59</v>
+      <c r="B16" s="85" t="s">
+        <v>101</v>
       </c>
       <c r="C16" s="36" t="s">
         <v>36</v>
@@ -3328,7 +3328,7 @@
       <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:256" customFormat="1" ht="27" customHeight="1">
-      <c r="B17" s="83"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="36" t="s">
         <v>39</v>
       </c>
@@ -3566,37 +3566,37 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:257" ht="30">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
       <c r="E6" s="48"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
       <c r="F7" s="3"/>
     </row>
     <row r="9" spans="1:257" ht="114">
       <c r="B9" s="66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:257" ht="71.25">
       <c r="B10" s="66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:257">
@@ -3842,31 +3842,31 @@
       <c r="F2" s="2"/>
     </row>
     <row r="4" spans="1:257" ht="30">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="1:257" ht="30.75" customHeight="1">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="33.75" customHeight="1">
@@ -3876,12 +3876,12 @@
     </row>
     <row r="9" spans="1:257" ht="409.5">
       <c r="B9" s="64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:257" ht="15">
       <c r="B11" s="58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:257" ht="15.75" thickBot="1">
@@ -3892,38 +3892,38 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:257" ht="15" thickBot="1">
-      <c r="B13" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="89" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="90"/>
+      <c r="B13" s="90" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="93"/>
       <c r="E13" s="61" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:257" ht="15" thickBot="1">
-      <c r="B14" s="88"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="62" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="62"/>
     </row>
     <row r="15" spans="1:257" s="1" customFormat="1" ht="99.75" customHeight="1" thickBot="1">
       <c r="A15" s="29"/>
       <c r="B15" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="62" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="62" t="s">
-        <v>64</v>
       </c>
       <c r="D15" s="62"/>
       <c r="E15" s="62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="24"/>
@@ -3934,14 +3934,14 @@
     <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A16" s="29"/>
       <c r="B16" s="63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="62"/>
       <c r="E16" s="62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="24"/>
@@ -3952,10 +3952,10 @@
     <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A17" s="29"/>
       <c r="B17" s="63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="62"/>
       <c r="E17" s="62"/>
@@ -3967,11 +3967,11 @@
     <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A18" s="29"/>
       <c r="B18" s="63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="62"/>
       <c r="D18" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="62"/>
       <c r="K18" s="15"/>
@@ -3981,10 +3981,10 @@
     <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="62"/>
       <c r="E19" s="62"/>
@@ -3993,38 +3993,38 @@
     <row r="20" spans="1:257" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
       <c r="A20" s="29"/>
       <c r="B20" s="63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="62"/>
       <c r="D20" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="IW20" s="2"/>
     </row>
     <row r="21" spans="1:257" s="1" customFormat="1" ht="66.75" customHeight="1" thickBot="1">
       <c r="A21" s="29"/>
       <c r="B21" s="63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="62"/>
       <c r="D21" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="IW21" s="2"/>
     </row>
     <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A22" s="29"/>
       <c r="B22" s="63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="62"/>
       <c r="E22" s="62"/>
@@ -4033,11 +4033,11 @@
     <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A23" s="29"/>
       <c r="B23" s="63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="62"/>
       <c r="D23" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="62"/>
       <c r="IW23" s="2"/>
@@ -4045,11 +4045,11 @@
     <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A24" s="29"/>
       <c r="B24" s="63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="62"/>
       <c r="D24" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" s="62"/>
       <c r="IW24" s="2"/>
@@ -4057,25 +4057,25 @@
     <row r="25" spans="1:257" s="1" customFormat="1" ht="66.75" customHeight="1" thickBot="1">
       <c r="A25" s="29"/>
       <c r="B25" s="63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="62"/>
       <c r="E25" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="IW25" s="2"/>
     </row>
     <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A26" s="29"/>
       <c r="B26" s="63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="62"/>
       <c r="D26" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="62"/>
       <c r="IW26" s="2"/>
@@ -4083,10 +4083,10 @@
     <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A27" s="29"/>
       <c r="B27" s="63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="62"/>
       <c r="E27" s="62"/>
@@ -4225,17 +4225,17 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="1:257" ht="30">
       <c r="B7" s="49" t="s">
@@ -4246,16 +4246,16 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="71"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79"/>
     </row>
     <row r="9" spans="1:257" ht="24.75" customHeight="1"/>
     <row r="10" spans="1:257" ht="409.5">
       <c r="B10" s="57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:257">
@@ -4496,32 +4496,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="71"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="71"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="79"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
@@ -4762,27 +4762,27 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:257" ht="30">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="79"/>
     </row>
     <row r="5" spans="1:257" ht="30">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="48"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="7" spans="1:257" ht="30">
       <c r="F7" s="3"/>

</xml_diff>